<commit_message>
adicionando dados do campeonato mundial de kite 2024
</commit_message>
<xml_diff>
--- a/data/mapeamento_competicoes_e_anos.xlsx
+++ b/data/mapeamento_competicoes_e_anos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Projetos\-sailing-rankings-2024.1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F7EA614-FD6B-4C73-85CA-D040AF1BE402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBB48C2-096A-443C-AE7B-B8F882DB066B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{090CE02F-83D2-45FF-8894-5F1D8D825D1E}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +124,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,13 +157,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B3E8C2-44DA-4B98-AEBA-0C214C5A93EA}">
-  <dimension ref="B2:M13"/>
+  <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,6 +810,9 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
       <c r="D11">
         <v>3</v>
       </c>
@@ -812,13 +824,16 @@
       </c>
       <c r="M11" s="2">
         <f>SUM(Tabela1[[#This Row],[2024]:[2015]])</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
       <c r="D12">
         <v>3</v>
       </c>
@@ -830,7 +845,7 @@
       </c>
       <c r="M12" s="2">
         <f>SUM(Tabela1[[#This Row],[2024]:[2015]])</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -839,7 +854,7 @@
       </c>
       <c r="C13" s="2">
         <f>SUM(C3:C12)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2">
         <f>SUM(D3:D12)</f>
@@ -879,8 +894,11 @@
       </c>
       <c r="M13" s="3">
         <f>SUM(Tabela1[[#This Row],[2024]:[2015]])</f>
-        <v>167</v>
-      </c>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
quase acabando a coleta dos dados da classe iqfoil de 2024 e atualizando as tabelas de competições
</commit_message>
<xml_diff>
--- a/data/mapeamento_competicoes_e_anos.xlsx
+++ b/data/mapeamento_competicoes_e_anos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Projetos\-sailing-rankings-2024.1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBB48C2-096A-443C-AE7B-B8F882DB066B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35B0502-C639-4A8F-B245-6CAA66002C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{090CE02F-83D2-45FF-8894-5F1D8D825D1E}"/>
   </bookViews>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B3E8C2-44DA-4B98-AEBA-0C214C5A93EA}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,6 +660,9 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="D5">
         <v>4</v>
       </c>
@@ -671,13 +674,16 @@
       </c>
       <c r="M5" s="2">
         <f>SUM(Tabela1[[#This Row],[2024]:[2015]])</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
       <c r="D6">
         <v>4</v>
       </c>
@@ -689,7 +695,7 @@
       </c>
       <c r="M6" s="2">
         <f>SUM(Tabela1[[#This Row],[2024]:[2015]])</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -854,7 +860,7 @@
       </c>
       <c r="C13" s="2">
         <f>SUM(C3:C12)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2">
         <f>SUM(D3:D12)</f>
@@ -894,16 +900,20 @@
       </c>
       <c r="M13" s="3">
         <f>SUM(Tabela1[[#This Row],[2024]:[2015]])</f>
-        <v>169</v>
-      </c>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="4"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>